<commit_message>
Update Ke hoach thuc hien Do An 1.xlsx
</commit_message>
<xml_diff>
--- a/Ke hoach thuc hien Do An 1.xlsx
+++ b/Ke hoach thuc hien Do An 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\3rd year\1st Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lequo\Documents\GitHub\-n-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267322A8-286E-4E8B-A894-01C4359AC041}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC5D57B-8C2D-403B-87DA-AE34B64F8D44}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -69,15 +66,6 @@
     <t>14/9/2018</t>
   </si>
   <si>
-    <t>26/9/2018</t>
-  </si>
-  <si>
-    <t>27/9/2018</t>
-  </si>
-  <si>
-    <t>20/9/2018</t>
-  </si>
-  <si>
     <t>Sinh viên thực hiện:</t>
   </si>
   <si>
@@ -93,33 +81,18 @@
     <t>Trần Phương Nam</t>
   </si>
   <si>
-    <t>BẢNG KẾ HOẠCH ĐỒ ÁN 1 Tên đồ án Phần mềm quản lí rạp chiếu phim</t>
-  </si>
-  <si>
     <t>Thiết kế form</t>
   </si>
   <si>
     <t>Thiết kế mô hình quan hệ ERD</t>
   </si>
   <si>
-    <t>Thu thập dữ liệu</t>
-  </si>
-  <si>
-    <t>Tạo Table</t>
-  </si>
-  <si>
-    <t>Viết báo cáo</t>
-  </si>
-  <si>
     <t>Thực thi và Chạy test</t>
   </si>
   <si>
     <t>Sửa lại nếu có sai sót</t>
   </si>
   <si>
-    <t>28/10/2018</t>
-  </si>
-  <si>
     <t>Tìm hiểu đồ án, lên kế hoạch</t>
   </si>
   <si>
@@ -132,10 +105,34 @@
     <t>24/11/2018</t>
   </si>
   <si>
-    <t>13/12/2018</t>
-  </si>
-  <si>
-    <t>15/12/2018</t>
+    <t>BẢNG KẾ HOẠCH ĐỒ ÁN 1: PHẦN MỀM QUẢN LÍ RẠP PHIM</t>
+  </si>
+  <si>
+    <t>22/10/2018</t>
+  </si>
+  <si>
+    <t>Viết đặc tả</t>
+  </si>
+  <si>
+    <t>Tạo bảng, Thêm dữ liệu vào các bảng</t>
+  </si>
+  <si>
+    <t>16/11/2018</t>
+  </si>
+  <si>
+    <t>Viết code cho các lớp</t>
+  </si>
+  <si>
+    <t>Tạo phần mềm theo mô hình 3 lớp sử dụng công nghệ ADO.NET</t>
+  </si>
+  <si>
+    <t>17/11/2018</t>
+  </si>
+  <si>
+    <t>Tổng kết, viết báo cáo</t>
+  </si>
+  <si>
+    <t>14/12/2018</t>
   </si>
 </sst>
 </file>
@@ -561,6 +558,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -582,21 +621,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -654,9 +681,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -692,33 +716,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1324,135 +1321,133 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7" style="5" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="58.140625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="35" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" style="15" hidden="1" customWidth="1"/>
-    <col min="7" max="10" width="25.85546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="10" width="25.85546875" style="7" customWidth="1"/>
     <col min="11" max="26" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="51" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="56"/>
-    </row>
-    <row r="2" spans="1:26" s="51" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="52" t="s">
+    <row r="1" spans="1:26" s="12" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:26" s="12" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
-    </row>
-    <row r="3" spans="1:26" s="51" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="50"/>
-    </row>
-    <row r="4" spans="1:26" s="51" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="50"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:26" s="12" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:26" s="12" customFormat="1" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:26" s="3" customFormat="1" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37">
+    <row r="6" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="46">
         <v>1</v>
       </c>
-      <c r="B6" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="31" t="s">
+      <c r="B6" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="27" t="s">
-        <v>29</v>
+      <c r="F6" s="29"/>
+      <c r="G6" s="37" t="s">
+        <v>27</v>
       </c>
       <c r="H6" s="57">
         <v>43142</v>
       </c>
-      <c r="I6" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="46"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="55"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1471,54 +1466,50 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="18" t="s">
+      <c r="B7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="58">
         <v>43170</v>
       </c>
       <c r="H7" s="58">
         <v>43231</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="28"/>
+      <c r="J7" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="44" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+    </row>
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="19" t="s">
+      <c r="B8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="36">
+      <c r="F8" s="29"/>
+      <c r="G8" s="45">
         <v>43262</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="45">
         <v>43292</v>
       </c>
-      <c r="I8" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="41"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1536,33 +1527,31 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
         <v>4</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="31" t="s">
+      <c r="B9" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="45">
+        <v>43262</v>
+      </c>
+      <c r="H9" s="45">
         <v>43292</v>
       </c>
-      <c r="H9" s="36">
-        <v>43323</v>
-      </c>
-      <c r="I9" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="43">
+      <c r="I9" s="45"/>
+      <c r="J9" s="52">
         <v>43200</v>
       </c>
       <c r="K9" s="2"/>
@@ -1583,80 +1572,78 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="31" t="s">
+      <c r="B10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="36">
-        <v>43354</v>
-      </c>
-      <c r="H10" s="36" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="45">
+        <v>43323</v>
+      </c>
+      <c r="H10" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="29"/>
+      <c r="J10" s="38"/>
+    </row>
+    <row r="11" spans="1:26" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>6</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="28"/>
-    </row>
-    <row r="11" spans="1:26" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="36">
-        <v>43324</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="28"/>
-    </row>
-    <row r="12" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="H11" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="J11" s="38"/>
+    </row>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
         <v>7</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="30" t="s">
+      <c r="B12" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="36">
-        <v>43355</v>
-      </c>
-      <c r="H12" s="36">
-        <v>43446</v>
-      </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="28"/>
+      <c r="G12" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="45">
+        <v>43112</v>
+      </c>
+      <c r="I12" s="29"/>
+      <c r="J12" s="38"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1674,29 +1661,31 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
         <v>8</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="32" t="s">
+      <c r="B13" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="45">
+        <v>43143</v>
+      </c>
+      <c r="H13" s="45">
+        <v>43385</v>
+      </c>
+      <c r="I13" s="29"/>
+      <c r="J13" s="38"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1714,19 +1703,29 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
         <v>9</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="28"/>
+      <c r="B14" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="45">
+        <v>43416</v>
+      </c>
+      <c r="H14" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="29"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1744,19 +1743,19 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
         <v>10</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="28"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="38"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1774,19 +1773,19 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+    <row r="16" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
         <v>11</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="28"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="38"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1805,34 +1804,34 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="20">
         <v>12</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="28"/>
-    </row>
-    <row r="18" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="38"/>
+    </row>
+    <row r="18" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
         <v>13</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="28"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="38"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1850,21 +1849,21 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+    <row r="19" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
         <v>14</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="28"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="38"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1882,21 +1881,21 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+    <row r="20" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
         <v>15</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="19" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="28"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="38"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1914,21 +1913,21 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+    <row r="21" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="23">
         <v>16</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="38"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1946,21 +1945,21 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+    <row r="22" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="23">
         <v>17</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="38"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1978,21 +1977,21 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" spans="1:26" s="11" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+    <row r="23" spans="1:26" s="4" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="23">
         <v>18</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="19" t="s">
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="28"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="38"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -2010,19 +2009,19 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37">
+    <row r="24" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="46">
         <v>19</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="41"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="50"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -2040,19 +2039,19 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37">
+    <row r="25" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="46">
         <v>20</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="41"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="50"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -2070,19 +2069,19 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" spans="1:26" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+    <row r="26" spans="1:26" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="29"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="39"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>

</xml_diff>